<commit_message>
change the parameter range seems can improve model simulation
</commit_message>
<xml_diff>
--- a/Matlab-code/tests for Jin/Matlab Code_For_Loren/Env_Variables_Output/Env_Variable_Master_Sheet.xlsx
+++ b/Matlab-code/tests for Jin/Matlab Code_For_Loren/Env_Variables_Output/Env_Variable_Master_Sheet.xlsx
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>